<commit_message>
Make it work with Handwriting
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Facultate\APB\UIPath-Project-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0CA5923-1D0A-40BE-9256-7F83B1837CA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A2DFBF4-6570-4CEF-A079-ACDCA3E70E6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8340" yWindow="2580" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="32">
   <si>
     <t>Data</t>
   </si>
@@ -85,6 +85,46 @@
   </si>
   <si>
     <t>Data Adaugare</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 500_x000D_
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13-11 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LOBODA </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 300_x000D_
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14-11 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> CEAPA </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 100_x000D_
+15-11 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 16-11 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> USTUROI </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 10_x000D_
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17-11 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> DOVLEAC </t>
   </si>
 </sst>
 </file>
@@ -120,11 +160,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -405,9 +448,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D90"/>
+  <dimension ref="A1:D101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
       <selection activeCell="D89" sqref="D89"/>
     </sheetView>
   </sheetViews>
@@ -1139,7 +1182,161 @@
         <v>500</v>
       </c>
       <c r="D90" s="1">
-        <v>44936.877129629633</v>
+        <v>44936</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" s="1">
+        <v>45270</v>
+      </c>
+      <c r="B91" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C91" s="2">
+        <v>500</v>
+      </c>
+      <c r="D91" s="1">
+        <v>44937</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A92" s="1">
+        <v>45270</v>
+      </c>
+      <c r="B92" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C92" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D92" s="1">
+        <v>44937</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A93" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B93" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C93" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D93" s="1">
+        <v>44937</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A94" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B94" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C94" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D94" s="1">
+        <v>44937</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A95" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B95" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C95" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D95" s="1">
+        <v>44937</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B96" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C96" s="2">
+        <v>5</v>
+      </c>
+      <c r="D96" s="1">
+        <v>44937</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A97" s="1">
+        <v>45270</v>
+      </c>
+      <c r="B97" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C97" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D97" s="1">
+        <v>44937.84</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A98" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B98" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C98" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D98" s="1">
+        <v>44937.84</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A99" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B99" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C99" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D99" s="1">
+        <v>44937.84</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A100" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B100" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C100" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D100" s="1">
+        <v>44937.84</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B101" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C101" s="2">
+        <v>5</v>
+      </c>
+      <c r="D101" s="1">
+        <v>44937.84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>